<commit_message>
Conteúdo de atualização: * Criação de proposta prototipação para consultas de histórico e proposta de tela de configuraçãod de regras (validar) * criação do documento de requisitos do sistema versão 2.0 * alteração da planilha de atividades baseline * Alteração de atribuição de responsável de atividades no dia 20/11 * criação do arquivo seguro.eap não oficial (cadastrado possiveis casos de uso (não detalhado pré e pós condições e nem passos alternativos, principais e de exceção) e digitado os requisitos e regras de negócio do sistema, conforme versão 2.0 do documento de requisitos)
</commit_message>
<xml_diff>
--- a/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_baseline.xlsx
+++ b/Docs/Planilha de atividades/Sistema_Seguradora_Planejamento_de_Atividades_baseline.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="89">
   <si>
     <t>Cód.</t>
   </si>
@@ -284,6 +284,9 @@
   <si>
     <t>Copia do Seguro.eap da sprint 2</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +345,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -401,6 +404,24 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -587,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,14 +778,21 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -772,16 +800,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,10 +1172,10 @@
   <dimension ref="A1:EE76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="AI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="AI39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="AW1" sqref="AW1"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="R13" sqref="R13"/>
+      <selection pane="bottomRight" activeCell="AO19" sqref="AO19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,181 +1268,181 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73">
+      <c r="D1" s="77">
         <v>42322</v>
       </c>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
       <c r="I1" s="13"/>
-      <c r="J1" s="73">
+      <c r="J1" s="77">
         <v>42323</v>
       </c>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
       <c r="O1" s="13"/>
-      <c r="P1" s="73">
+      <c r="P1" s="77">
         <v>42324</v>
       </c>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
       <c r="U1" s="13"/>
-      <c r="V1" s="73">
+      <c r="V1" s="77">
         <v>42325</v>
       </c>
-      <c r="W1" s="74"/>
-      <c r="X1" s="74"/>
-      <c r="Y1" s="74"/>
-      <c r="Z1" s="74"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
       <c r="AA1" s="13"/>
-      <c r="AB1" s="73">
+      <c r="AB1" s="77">
         <v>42326</v>
       </c>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="74"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
       <c r="AG1" s="13"/>
-      <c r="AH1" s="73">
+      <c r="AH1" s="77">
         <v>42327</v>
       </c>
-      <c r="AI1" s="74"/>
-      <c r="AJ1" s="74"/>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="78"/>
+      <c r="AK1" s="78"/>
+      <c r="AL1" s="78"/>
       <c r="AM1" s="13"/>
-      <c r="AN1" s="73">
+      <c r="AN1" s="77">
         <v>42328</v>
       </c>
-      <c r="AO1" s="74"/>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="74"/>
-      <c r="AR1" s="74"/>
+      <c r="AO1" s="78"/>
+      <c r="AP1" s="78"/>
+      <c r="AQ1" s="78"/>
+      <c r="AR1" s="78"/>
       <c r="AS1" s="13"/>
-      <c r="AT1" s="73">
+      <c r="AT1" s="77">
         <v>42329</v>
       </c>
-      <c r="AU1" s="74"/>
-      <c r="AV1" s="74"/>
-      <c r="AW1" s="74"/>
-      <c r="AX1" s="74"/>
+      <c r="AU1" s="78"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="78"/>
+      <c r="AX1" s="78"/>
       <c r="AY1" s="13"/>
-      <c r="AZ1" s="73">
+      <c r="AZ1" s="77">
         <v>42330</v>
       </c>
-      <c r="BA1" s="74"/>
-      <c r="BB1" s="74"/>
-      <c r="BC1" s="74"/>
-      <c r="BD1" s="74"/>
+      <c r="BA1" s="78"/>
+      <c r="BB1" s="78"/>
+      <c r="BC1" s="78"/>
+      <c r="BD1" s="78"/>
       <c r="BE1" s="13"/>
-      <c r="BF1" s="73">
+      <c r="BF1" s="77">
         <v>42331</v>
       </c>
-      <c r="BG1" s="74"/>
-      <c r="BH1" s="74"/>
-      <c r="BI1" s="74"/>
-      <c r="BJ1" s="74"/>
+      <c r="BG1" s="78"/>
+      <c r="BH1" s="78"/>
+      <c r="BI1" s="78"/>
+      <c r="BJ1" s="78"/>
       <c r="BK1" s="13"/>
-      <c r="BL1" s="73">
+      <c r="BL1" s="77">
         <v>42332</v>
       </c>
-      <c r="BM1" s="74"/>
-      <c r="BN1" s="74"/>
-      <c r="BO1" s="74"/>
-      <c r="BP1" s="74"/>
+      <c r="BM1" s="78"/>
+      <c r="BN1" s="78"/>
+      <c r="BO1" s="78"/>
+      <c r="BP1" s="78"/>
       <c r="BQ1" s="13"/>
-      <c r="BR1" s="73">
+      <c r="BR1" s="77">
         <v>42333</v>
       </c>
-      <c r="BS1" s="74"/>
-      <c r="BT1" s="74"/>
-      <c r="BU1" s="74"/>
-      <c r="BV1" s="74"/>
+      <c r="BS1" s="78"/>
+      <c r="BT1" s="78"/>
+      <c r="BU1" s="78"/>
+      <c r="BV1" s="78"/>
       <c r="BW1" s="13"/>
-      <c r="BX1" s="73">
+      <c r="BX1" s="77">
         <v>42334</v>
       </c>
-      <c r="BY1" s="74"/>
-      <c r="BZ1" s="74"/>
-      <c r="CA1" s="74"/>
-      <c r="CB1" s="74"/>
+      <c r="BY1" s="78"/>
+      <c r="BZ1" s="78"/>
+      <c r="CA1" s="78"/>
+      <c r="CB1" s="78"/>
       <c r="CC1" s="13"/>
-      <c r="CD1" s="73">
+      <c r="CD1" s="77">
         <v>42335</v>
       </c>
-      <c r="CE1" s="74"/>
-      <c r="CF1" s="74"/>
-      <c r="CG1" s="74"/>
-      <c r="CH1" s="74"/>
+      <c r="CE1" s="78"/>
+      <c r="CF1" s="78"/>
+      <c r="CG1" s="78"/>
+      <c r="CH1" s="78"/>
       <c r="CI1" s="13"/>
-      <c r="CJ1" s="73">
+      <c r="CJ1" s="77">
         <v>42336</v>
       </c>
-      <c r="CK1" s="74"/>
-      <c r="CL1" s="74"/>
-      <c r="CM1" s="74"/>
-      <c r="CN1" s="74"/>
+      <c r="CK1" s="78"/>
+      <c r="CL1" s="78"/>
+      <c r="CM1" s="78"/>
+      <c r="CN1" s="78"/>
       <c r="CO1" s="13"/>
-      <c r="CP1" s="73">
+      <c r="CP1" s="77">
         <v>42337</v>
       </c>
-      <c r="CQ1" s="74"/>
-      <c r="CR1" s="74"/>
-      <c r="CS1" s="74"/>
-      <c r="CT1" s="74"/>
+      <c r="CQ1" s="78"/>
+      <c r="CR1" s="78"/>
+      <c r="CS1" s="78"/>
+      <c r="CT1" s="78"/>
       <c r="CU1" s="13"/>
-      <c r="CV1" s="73">
+      <c r="CV1" s="77">
         <v>42338</v>
       </c>
-      <c r="CW1" s="74"/>
-      <c r="CX1" s="74"/>
-      <c r="CY1" s="74"/>
-      <c r="CZ1" s="74"/>
+      <c r="CW1" s="78"/>
+      <c r="CX1" s="78"/>
+      <c r="CY1" s="78"/>
+      <c r="CZ1" s="78"/>
       <c r="DA1" s="13"/>
-      <c r="DB1" s="73">
+      <c r="DB1" s="77">
         <v>42339</v>
       </c>
-      <c r="DC1" s="74"/>
-      <c r="DD1" s="74"/>
-      <c r="DE1" s="74"/>
-      <c r="DF1" s="74"/>
+      <c r="DC1" s="78"/>
+      <c r="DD1" s="78"/>
+      <c r="DE1" s="78"/>
+      <c r="DF1" s="78"/>
       <c r="DG1" s="13"/>
-      <c r="DH1" s="73">
+      <c r="DH1" s="77">
         <v>42340</v>
       </c>
-      <c r="DI1" s="74"/>
-      <c r="DJ1" s="74"/>
-      <c r="DK1" s="74"/>
-      <c r="DL1" s="74"/>
+      <c r="DI1" s="78"/>
+      <c r="DJ1" s="78"/>
+      <c r="DK1" s="78"/>
+      <c r="DL1" s="78"/>
       <c r="DM1" s="13"/>
-      <c r="DN1" s="73">
+      <c r="DN1" s="77">
         <v>42341</v>
       </c>
-      <c r="DO1" s="74"/>
-      <c r="DP1" s="74"/>
-      <c r="DQ1" s="74"/>
-      <c r="DR1" s="74"/>
+      <c r="DO1" s="78"/>
+      <c r="DP1" s="78"/>
+      <c r="DQ1" s="78"/>
+      <c r="DR1" s="78"/>
       <c r="DS1" s="13"/>
-      <c r="DT1" s="73">
+      <c r="DT1" s="77">
         <v>42342</v>
       </c>
-      <c r="DU1" s="74"/>
-      <c r="DV1" s="74"/>
-      <c r="DW1" s="74"/>
-      <c r="DX1" s="74"/>
+      <c r="DU1" s="78"/>
+      <c r="DV1" s="78"/>
+      <c r="DW1" s="78"/>
+      <c r="DX1" s="78"/>
       <c r="DY1" s="13"/>
-      <c r="DZ1" s="73">
+      <c r="DZ1" s="77">
         <v>42343</v>
       </c>
-      <c r="EA1" s="74"/>
-      <c r="EB1" s="74"/>
-      <c r="EC1" s="74"/>
-      <c r="ED1" s="74"/>
+      <c r="EA1" s="78"/>
+      <c r="EB1" s="78"/>
+      <c r="EC1" s="78"/>
+      <c r="ED1" s="78"/>
       <c r="EE1" s="13"/>
     </row>
     <row r="2" spans="1:135" ht="45" customHeight="1">
@@ -2567,7 +2591,7 @@
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="76" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="15">
@@ -2717,7 +2741,7 @@
       <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="75"/>
+      <c r="C9" s="76"/>
       <c r="D9" s="7">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -2867,7 +2891,7 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="78" t="s">
+      <c r="C10" s="75" t="s">
         <v>71</v>
       </c>
       <c r="D10" s="7">
@@ -3017,7 +3041,7 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="75"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="7">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3165,7 +3189,7 @@
       <c r="B12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="78" t="s">
+      <c r="C12" s="75" t="s">
         <v>72</v>
       </c>
       <c r="D12" s="7">
@@ -3317,7 +3341,7 @@
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="75"/>
+      <c r="C13" s="76"/>
       <c r="D13" s="7">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3465,7 +3489,7 @@
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="75"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="7">
         <v>4.1666666666666699E-2</v>
       </c>
@@ -3632,7 +3656,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="9"/>
       <c r="S15" s="10"/>
-      <c r="T15" s="81"/>
+      <c r="T15" s="73"/>
       <c r="U15" s="13"/>
       <c r="V15" s="7"/>
       <c r="W15" s="8"/>
@@ -4089,7 +4113,7 @@
       <c r="AO18" s="8"/>
       <c r="AP18" s="9"/>
       <c r="AQ18" s="10"/>
-      <c r="AR18" s="43"/>
+      <c r="AR18" s="84"/>
       <c r="AS18" s="13"/>
       <c r="AT18" s="7"/>
       <c r="AU18" s="8"/>
@@ -4232,7 +4256,7 @@
       <c r="AO19" s="8"/>
       <c r="AP19" s="9"/>
       <c r="AQ19" s="10"/>
-      <c r="AR19" s="43"/>
+      <c r="AR19" s="84"/>
       <c r="AS19" s="13"/>
       <c r="AT19" s="7"/>
       <c r="AU19" s="8"/>
@@ -4371,11 +4395,13 @@
       <c r="AK20" s="10"/>
       <c r="AL20" s="11"/>
       <c r="AM20" s="13"/>
-      <c r="AN20" s="58"/>
+      <c r="AN20" s="58">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="AO20" s="8"/>
       <c r="AP20" s="9"/>
       <c r="AQ20" s="10"/>
-      <c r="AR20" s="43"/>
+      <c r="AR20" s="82"/>
       <c r="AS20" s="13"/>
       <c r="AT20" s="7"/>
       <c r="AU20" s="8"/>
@@ -4947,11 +4973,13 @@
       <c r="AK24" s="10"/>
       <c r="AL24" s="11"/>
       <c r="AM24" s="13"/>
-      <c r="AN24" s="58"/>
+      <c r="AN24" s="58">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="AO24" s="8"/>
       <c r="AP24" s="9"/>
       <c r="AQ24" s="10"/>
-      <c r="AR24" s="43"/>
+      <c r="AR24" s="83"/>
       <c r="AS24" s="13"/>
       <c r="AT24" s="7"/>
       <c r="AU24" s="8"/>
@@ -5053,7 +5081,7 @@
       <c r="B25" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="76" t="s">
+      <c r="C25" s="79" t="s">
         <v>23</v>
       </c>
       <c r="D25" s="7"/>
@@ -5198,7 +5226,7 @@
       <c r="B26" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="77"/>
+      <c r="C26" s="80"/>
       <c r="D26" s="7"/>
       <c r="E26" s="8"/>
       <c r="F26" s="9"/>
@@ -5627,7 +5655,7 @@
       <c r="B29" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="76" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="7"/>
@@ -5772,7 +5800,7 @@
       <c r="B30" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C30" s="75"/>
+      <c r="C30" s="76"/>
       <c r="D30" s="7"/>
       <c r="E30" s="8"/>
       <c r="F30" s="9"/>
@@ -5915,7 +5943,7 @@
       <c r="B31" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="75"/>
+      <c r="C31" s="76"/>
       <c r="D31" s="7"/>
       <c r="E31" s="8"/>
       <c r="F31" s="9"/>
@@ -6777,7 +6805,7 @@
       <c r="B37" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="76" t="s">
         <v>14</v>
       </c>
       <c r="D37" s="7"/>
@@ -6922,7 +6950,7 @@
       <c r="B38" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="75"/>
+      <c r="C38" s="76"/>
       <c r="D38" s="7"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9"/>
@@ -8250,7 +8278,7 @@
       <c r="AO47" s="8"/>
       <c r="AP47" s="9"/>
       <c r="AQ47" s="10"/>
-      <c r="AR47" s="54"/>
+      <c r="AR47" s="55"/>
       <c r="AS47" s="13"/>
       <c r="AT47" s="7"/>
       <c r="AU47" s="8"/>
@@ -8363,7 +8391,9 @@
       <c r="K48" s="19"/>
       <c r="L48" s="19"/>
       <c r="M48" s="19"/>
-      <c r="N48" s="11"/>
+      <c r="N48" s="11" t="s">
+        <v>88</v>
+      </c>
       <c r="O48" s="13"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="19"/>
@@ -8522,13 +8552,11 @@
       <c r="G49" s="19"/>
       <c r="H49" s="11"/>
       <c r="I49" s="13"/>
-      <c r="J49" s="15">
-        <v>8.3333333333333329E-2</v>
-      </c>
+      <c r="J49" s="15"/>
       <c r="K49" s="19"/>
       <c r="L49" s="19"/>
       <c r="M49" s="19"/>
-      <c r="N49" s="56"/>
+      <c r="N49" s="73"/>
       <c r="O49" s="13"/>
       <c r="P49" s="15"/>
       <c r="Q49" s="19"/>
@@ -8841,7 +8869,7 @@
       <c r="B51" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="79" t="s">
+      <c r="C51" s="74" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="15"/>
@@ -8984,7 +9012,7 @@
       <c r="B52" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="79"/>
+      <c r="C52" s="74"/>
       <c r="D52" s="15"/>
       <c r="E52" s="19"/>
       <c r="F52" s="9"/>
@@ -9840,7 +9868,7 @@
       <c r="B58" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C58" s="79" t="s">
+      <c r="C58" s="74" t="s">
         <v>30</v>
       </c>
       <c r="D58" s="15"/>
@@ -9983,7 +10011,7 @@
       <c r="B59" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C59" s="79"/>
+      <c r="C59" s="74"/>
       <c r="D59" s="15"/>
       <c r="E59" s="19"/>
       <c r="F59" s="19"/>
@@ -10124,7 +10152,7 @@
       <c r="B60" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C60" s="79"/>
+      <c r="C60" s="74"/>
       <c r="D60" s="15"/>
       <c r="E60" s="19"/>
       <c r="F60" s="19"/>
@@ -10823,7 +10851,7 @@
       <c r="H64" s="32"/>
       <c r="J64" s="29">
         <f>SUM(J3:J61)</f>
-        <v>0.125</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="K64" s="30">
         <f>SUM(K3:K61)</f>
@@ -10903,7 +10931,7 @@
       <c r="AL64" s="32"/>
       <c r="AN64" s="29">
         <f>SUM(AN3:AN61)</f>
-        <v>0.37499999999999994</v>
+        <v>0.54166666666666674</v>
       </c>
       <c r="AO64" s="30">
         <f>SUM(AO3:AO61)</f>
@@ -12252,22 +12280,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D1:H1"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="DN1:DR1"/>
-    <mergeCell ref="DT1:DX1"/>
     <mergeCell ref="DZ1:ED1"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C25:C26"/>
@@ -12282,6 +12294,22 @@
     <mergeCell ref="BX1:CB1"/>
     <mergeCell ref="CD1:CH1"/>
     <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="DN1:DR1"/>
+    <mergeCell ref="DT1:DX1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="C10:C11"/>
   </mergeCells>
   <pageMargins left="0.23611111111111099" right="0.23611111111111099" top="0.35416666666666702" bottom="0.35416666666666702" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -12363,18 +12391,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="80"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="39" t="s">

</xml_diff>